<commit_message>
Final submission for gridded/randomized closest point
</commit_message>
<xml_diff>
--- a/Project3/Running_Times_Data.xlsx
+++ b/Project3/Running_Times_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgagv\OneDrive\Documents\ComputerVision\Project3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973EEE63-0A28-4F7E-B329-4AC2564A11FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F00C5BA-3123-4580-A2FF-1108224721EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="9420" xr2:uid="{0A0AA3E2-E972-4405-B191-F828A643A39C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{0A0AA3E2-E972-4405-B191-F828A643A39C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -234,10 +234,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$9</c:f>
+              <c:f>Sheet1!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>50000</c:v>
                 </c:pt>
@@ -261,16 +261,22 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>750000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$9</c:f>
+              <c:f>Sheet1!$C$2:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>17</c:v>
                 </c:pt>
@@ -359,10 +365,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$9</c:f>
+              <c:f>Sheet1!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>50000</c:v>
                 </c:pt>
@@ -386,16 +392,22 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>750000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$9</c:f>
+              <c:f>Sheet1!$D$2:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>15</c:v>
                 </c:pt>
@@ -419,6 +431,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>827</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1568</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -427,6 +442,942 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-F04E-40AF-A17E-59E2AF20FEA9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time (Gridded)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent3">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>750000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AD45-4CC1-8417-61A48E19A5FC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1174377535"/>
+        <c:axId val="1174360063"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1174377535"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of points</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:noFill/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1174360063"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1174360063"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (Seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1174377535"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Closest</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Point Problem - Algorithm Comparison</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time (Brute Force)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>750000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>319</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>405</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>808</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1175</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A409-408E-A315-4321FE99F56B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time (Recursive)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>750000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>207</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>281</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>342</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>827</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1568</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A409-408E-A315-4321FE99F56B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time (Gridded)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent3">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>750000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A409-408E-A315-4321FE99F56B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -788,6 +1739,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
@@ -1326,20 +2317,558 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>198120</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>206141</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>15641</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>502920</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>510941</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>15641</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1359,6 +2888,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A45E120-2EA4-47EA-9A54-E20CA917B1B6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1664,10 +3231,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A34AEE8-5268-481D-B785-0160E9296BF6}">
-  <dimension ref="B1:E9"/>
+  <dimension ref="B1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1701,6 +3268,9 @@
       <c r="D2">
         <v>15</v>
       </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3">
@@ -1712,6 +3282,9 @@
       <c r="D3">
         <v>26</v>
       </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4">
@@ -1723,6 +3296,9 @@
       <c r="D4">
         <v>69</v>
       </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5">
@@ -1734,6 +3310,9 @@
       <c r="D5">
         <v>97</v>
       </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6">
@@ -1745,6 +3324,9 @@
       <c r="D6">
         <v>207</v>
       </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7">
@@ -1756,6 +3338,9 @@
       <c r="D7">
         <v>281</v>
       </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8">
@@ -1767,6 +3352,9 @@
       <c r="D8">
         <v>342</v>
       </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9">
@@ -1777,6 +3365,28 @@
       </c>
       <c r="D9">
         <v>827</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>750000</v>
+      </c>
+      <c r="D10">
+        <v>1568</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>1000000</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>